<commit_message>
impresion calidad y ajuste de . , en campo ancho
</commit_message>
<xml_diff>
--- a/nueva_bobina.xlsx
+++ b/nueva_bobina.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2872,6 +2872,1146 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>25/08/2025 10:40</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>COVERING</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>25/08/2025 10:41</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>COVERING</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>25/08/2025 10:43</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>COVERING</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>25/08/2025 10:48</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>COVERING</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>25/08/2025 10:48</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>COVERING</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>1211</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>25/08/2025 10:51</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>511</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>15444</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>5454</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>25/08/2025 10:55</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>CART.GRIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>545</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>4544</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>4444</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>25/08/2025 11:00</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>545</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>4544</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>4444</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>25/08/2025 11:03</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>560</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>54545</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>21215</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>25/08/2025 11:29</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>544</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>1245</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>45455</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:33</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>544</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>12154</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>4545</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:36</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>L.BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>254</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>5455</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>4455</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:38</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>CART.BLANCA</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>544</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>45454</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:40</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>CART.BLANCA</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>1501</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>22454</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:42</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>ONDA LINER</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>545</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>45578</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>88877</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:44</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>CART.BLANCA</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>545</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>45578</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>88877</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:44</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>ONDA LINER</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>62,5</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2455</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>4455</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>5544</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:47</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>CART.BLANCA</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>62,5</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>5444</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>5454</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>54545</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:48</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>CART.BLANCA</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>62,5</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>5444</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>5454</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>54545</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>26/08/2025 08:49</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>ONDA LINER</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>